<commit_message>
maj feuilles Excel (consommation gaz/électricité: Mars/avril 2017)
</commit_message>
<xml_diff>
--- a/Tableau_Electricite.xlsx
+++ b/Tableau_Electricite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etienne\OpenClassrooms\Gérez code avec Git &amp; GitHub (cours)\Activites\activite1\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etienne\OpenClassrooms\github\activite1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,18 +749,20 @@
       <c r="B4" s="3">
         <v>85.21</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>107.55</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6">
         <f t="shared" si="0"/>
-        <v>85.21</v>
+        <v>192.76</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" si="1"/>
-        <v>7.1008333333333331</v>
+        <v>16.063333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>